<commit_message>
SML Experiment for the paper 7/5/2024
</commit_message>
<xml_diff>
--- a/Python/features/DatasetRandomTreeClassificationResults.xlsx
+++ b/Python/features/DatasetRandomTreeClassificationResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebApriori\Python\features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\WebApriori\Python\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11AD887-3CD4-4B37-AA60-729C2D160A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51220459-5F75-4A64-829A-11AEB6F10648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{2F99A6A5-D16C-4B5D-A6A4-D283C14BE1EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F99A6A5-D16C-4B5D-A6A4-D283C14BE1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
   <si>
     <t>K-fold 3</t>
   </si>
@@ -98,6 +98,24 @@
   <si>
     <t>92.6%</t>
   </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Training V5</t>
+  </si>
+  <si>
+    <t>Training V1</t>
+  </si>
+  <si>
+    <t>SVM RBF Kernel 
+C=1, gamma=0,3</t>
+  </si>
+  <si>
+    <t>KNN Classifier
+neighbors=2
+C=1, gamma=0,3</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -377,6 +401,7 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -401,25 +426,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -751,31 +787,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062EC006-8C97-47AC-BD32-415DF786C586}">
-  <dimension ref="A1:T104"/>
+  <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="P61" sqref="P61:Q74"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="21"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="22"/>
+      <c r="V1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="23"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="24"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="24"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -824,8 +866,14 @@
       <c r="Q3" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.85799999999999998</v>
       </c>
@@ -849,13 +897,19 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P4" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="V4" s="10">
         <v>0.95299999999999996</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="W4" s="11">
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.89200000000000002</v>
       </c>
@@ -876,11 +930,15 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="P5" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="V5" s="10">
         <v>0.90400000000000003</v>
       </c>
-      <c r="Q5" s="11"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.95</v>
       </c>
@@ -901,11 +959,15 @@
         <v>0.92400000000000004</v>
       </c>
       <c r="P6" s="10">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="V6" s="10">
         <v>0.90300000000000002</v>
       </c>
-      <c r="Q6" s="11"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.85799999999999998</v>
       </c>
@@ -926,11 +988,15 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="P7" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="Q7" s="11"/>
+      <c r="V7" s="10">
         <v>0.95199999999999996</v>
       </c>
-      <c r="Q7" s="11"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.90800000000000003</v>
       </c>
@@ -951,11 +1017,15 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="P8" s="10">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="Q8" s="11"/>
+      <c r="V8" s="10">
         <v>0.871</v>
       </c>
-      <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.89200000000000002</v>
       </c>
@@ -976,11 +1046,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P9" s="10">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="V9" s="10">
         <v>0.92700000000000005</v>
       </c>
-      <c r="Q9" s="11"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.90800000000000003</v>
       </c>
@@ -1001,11 +1075,15 @@
         <v>0.91600000000000004</v>
       </c>
       <c r="P10" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="V10" s="10">
         <v>0.94199999999999995</v>
       </c>
-      <c r="Q10" s="11"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W10" s="11"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.86699999999999999</v>
       </c>
@@ -1026,11 +1104,15 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="P11" s="10">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="V11" s="10">
         <v>0.91200000000000003</v>
       </c>
-      <c r="Q11" s="11"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.875</v>
       </c>
@@ -1051,11 +1133,15 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="P12" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="V12" s="10">
         <v>0.91800000000000004</v>
       </c>
-      <c r="Q12" s="11"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W12" s="11"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.91700000000000004</v>
       </c>
@@ -1076,11 +1162,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P13" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q13" s="11"/>
+      <c r="V13" s="10">
         <v>0.91200000000000003</v>
       </c>
-      <c r="Q13" s="11"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" ref="A14" si="0">AVERAGE(A4:A13)</f>
         <v>0.89250000000000007</v>
@@ -1137,30 +1227,44 @@
         <f t="shared" ref="N14" si="12">AVERAGE(N4:N13)</f>
         <v>0.91700000000000004</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="13">
         <f t="shared" ref="P14:Q14" si="13">AVERAGE(P4:P13)</f>
-        <v>0.91940000000000011</v>
+        <v>0.79430000000000001</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="13"/>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="V14" s="12">
+        <f t="shared" ref="V14:W14" si="14">AVERAGE(V4:V13)</f>
+        <v>0.91940000000000011</v>
+      </c>
+      <c r="W14" s="13">
+        <f t="shared" si="14"/>
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P16" s="16" t="s">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="17"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q16" s="18"/>
+      <c r="V16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="W16" s="18"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="19"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P17" s="19"/>
+      <c r="Q17" s="20"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="20"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
@@ -1209,8 +1313,14 @@
       <c r="Q18" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.90800000000000003</v>
       </c>
@@ -1254,13 +1364,19 @@
         <v>0.94199999999999995</v>
       </c>
       <c r="P19" s="10">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="V19" s="10">
         <v>0.83599999999999997</v>
       </c>
-      <c r="Q19" s="11">
+      <c r="W19" s="11">
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.91700000000000004</v>
       </c>
@@ -1301,11 +1417,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P20" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q20" s="11"/>
+      <c r="V20" s="10">
         <v>0.83199999999999996</v>
       </c>
-      <c r="Q20" s="11"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.91700000000000004</v>
       </c>
@@ -1346,11 +1466,15 @@
         <v>0.93299999999999994</v>
       </c>
       <c r="P21" s="10">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="V21" s="10">
         <v>0.83099999999999996</v>
       </c>
-      <c r="Q21" s="11"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.88300000000000001</v>
       </c>
@@ -1391,11 +1515,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P22" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q22" s="11"/>
+      <c r="V22" s="10">
         <v>0.84699999999999998</v>
       </c>
-      <c r="Q22" s="11"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.9</v>
       </c>
@@ -1436,11 +1564,15 @@
         <v>0.94200000000000006</v>
       </c>
       <c r="P23" s="10">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="V23" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="Q23" s="11"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.9</v>
       </c>
@@ -1481,11 +1613,15 @@
         <v>0.94200000000000006</v>
       </c>
       <c r="P24" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="V24" s="10">
         <v>0.83899999999999997</v>
       </c>
-      <c r="Q24" s="11"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.95</v>
       </c>
@@ -1526,11 +1662,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P25" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="V25" s="10">
         <v>0.83899999999999997</v>
       </c>
-      <c r="Q25" s="11"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0.88300000000000001</v>
       </c>
@@ -1571,11 +1711,15 @@
         <v>0.90799999999999992</v>
       </c>
       <c r="P26" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q26" s="11"/>
+      <c r="V26" s="10">
         <v>0.84599999999999997</v>
       </c>
-      <c r="Q26" s="11"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0.85</v>
       </c>
@@ -1616,11 +1760,15 @@
         <v>0.94200000000000006</v>
       </c>
       <c r="P27" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="Q27" s="11"/>
+      <c r="V27" s="10">
         <v>0.81499999999999995</v>
       </c>
-      <c r="Q27" s="11"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0.92500000000000004</v>
       </c>
@@ -1661,29 +1809,33 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="P28" s="10">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="Q28" s="11"/>
+      <c r="V28" s="10">
         <v>0.84699999999999998</v>
       </c>
-      <c r="Q28" s="11"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" ref="A29:E29" si="14">AVERAGE(A19:A28)</f>
+        <f t="shared" ref="A29:E29" si="15">AVERAGE(A19:A28)</f>
         <v>0.9033000000000001</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.91580000000000017</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.91920000000000002</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.91320000000000001</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.91670000000000018</v>
       </c>
       <c r="F29" s="2">
@@ -1691,57 +1843,69 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" ref="G29:N29" si="15">AVERAGE(G19:G28)</f>
+        <f t="shared" ref="G29:N29" si="16">AVERAGE(G19:G28)</f>
         <v>0.92400000000000004</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.91830000000000012</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.91899999999999993</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.9225000000000001</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.92899999999999994</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.92739999999999989</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.92759999999999998</v>
       </c>
       <c r="N29" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.94199999999999995</v>
       </c>
       <c r="P29" s="12">
-        <f t="shared" ref="P29:Q29" si="16">AVERAGE(P19:P28)</f>
+        <f t="shared" ref="P29:Q29" si="17">AVERAGE(P19:P28)</f>
+        <v>0.7734000000000002</v>
+      </c>
+      <c r="Q29" s="13">
+        <f t="shared" si="17"/>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="V29" s="12">
+        <f t="shared" ref="V29:W29" si="18">AVERAGE(V19:V28)</f>
         <v>0.83399999999999996</v>
       </c>
-      <c r="Q29" s="13">
-        <f t="shared" si="16"/>
+      <c r="W29" s="13">
+        <f t="shared" si="18"/>
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="P31" s="16" t="s">
+      <c r="P31" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Q31" s="17"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31" s="18"/>
+      <c r="V31" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="W31" s="18"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>0</v>
       </c>
@@ -1784,10 +1948,12 @@
       <c r="N32" s="5">
         <v>120</v>
       </c>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="19"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P32" s="19"/>
+      <c r="Q32" s="20"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="20"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0.89700000000000002</v>
       </c>
@@ -1836,8 +2002,14 @@
       <c r="Q33" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W33" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0.88300000000000001</v>
       </c>
@@ -1878,13 +2050,19 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="P34" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="V34" s="10">
         <v>0.94299999999999995</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="W34" s="11">
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0.90800000000000003</v>
       </c>
@@ -1925,11 +2103,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P35" s="10">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="Q35" s="11"/>
+      <c r="V35" s="10">
         <v>0.94399999999999995</v>
       </c>
-      <c r="Q35" s="11"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W35" s="11"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>0.89100000000000001</v>
       </c>
@@ -1970,11 +2152,15 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="P36" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="Q36" s="11"/>
+      <c r="V36" s="10">
         <v>0.96699999999999997</v>
       </c>
-      <c r="Q36" s="11"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W36" s="11"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0.92500000000000004</v>
       </c>
@@ -2015,11 +2201,15 @@
         <v>0.94200000000000006</v>
       </c>
       <c r="P37" s="10">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="Q37" s="11"/>
+      <c r="V37" s="10">
         <v>0.96899999999999997</v>
       </c>
-      <c r="Q37" s="11"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W37" s="11"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0.90800000000000003</v>
       </c>
@@ -2060,11 +2250,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P38" s="10">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="Q38" s="11"/>
+      <c r="V38" s="10">
         <v>0.96799999999999997</v>
       </c>
-      <c r="Q38" s="11"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W38" s="11"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>0.91700000000000004</v>
       </c>
@@ -2105,11 +2299,15 @@
         <v>0.93299999999999994</v>
       </c>
       <c r="P39" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="Q39" s="11"/>
+      <c r="V39" s="10">
         <v>0.94199999999999995</v>
       </c>
-      <c r="Q39" s="11"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W39" s="11"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>0.88300000000000001</v>
       </c>
@@ -2150,11 +2348,15 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="P40" s="10">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="Q40" s="11"/>
+      <c r="V40" s="10">
         <v>0.95099999999999996</v>
       </c>
-      <c r="Q40" s="11"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W40" s="11"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>0.9</v>
       </c>
@@ -2195,11 +2397,15 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="P41" s="10">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="Q41" s="11"/>
+      <c r="V41" s="10">
         <v>0.96699999999999997</v>
       </c>
-      <c r="Q41" s="11"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W41" s="11"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>0.93300000000000005</v>
       </c>
@@ -2240,88 +2446,104 @@
         <v>0.94200000000000006</v>
       </c>
       <c r="P42" s="10">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="Q42" s="11"/>
+      <c r="V42" s="10">
         <v>0.95299999999999996</v>
       </c>
-      <c r="Q42" s="11"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W42" s="11"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f>AVERAGE(A33:A42)</f>
         <v>0.90449999999999997</v>
       </c>
       <c r="B43" s="2">
-        <f t="shared" ref="B43:N43" si="17">AVERAGE(B33:B42)</f>
+        <f t="shared" ref="B43:N43" si="19">AVERAGE(B33:B42)</f>
         <v>0.91389999999999993</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91630000000000023</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91460000000000008</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91600000000000015</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.92430000000000001</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91969999999999996</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91940000000000011</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91899999999999993</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.91840000000000011</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.92970000000000008</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.92389999999999994</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.92759999999999998</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.93299999999999994</v>
       </c>
       <c r="P43" s="10">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="Q43" s="11"/>
+      <c r="V43" s="10">
         <v>0.96899999999999997</v>
       </c>
-      <c r="Q43" s="11"/>
-    </row>
-    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W43" s="11"/>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P44" s="12">
-        <f t="shared" ref="P44:Q44" si="18">AVERAGE(P34:P43)</f>
+        <f t="shared" ref="P44:Q44" si="20">AVERAGE(P34:P43)</f>
+        <v>0.86009999999999986</v>
+      </c>
+      <c r="Q44" s="13">
+        <f t="shared" si="20"/>
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="V44" s="12">
+        <f t="shared" ref="V44:W44" si="21">AVERAGE(V34:V43)</f>
         <v>0.95729999999999982</v>
       </c>
-      <c r="Q44" s="13">
-        <f t="shared" si="18"/>
+      <c r="W44" s="13">
+        <f t="shared" si="21"/>
         <v>0.96299999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>0</v>
       </c>
@@ -2364,16 +2586,24 @@
       <c r="N46" s="5">
         <v>124</v>
       </c>
-      <c r="P46" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q46" s="17"/>
-      <c r="S46" s="16" t="s">
+      <c r="P46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q46" s="18"/>
+      <c r="S46" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="T46" s="17"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T46" s="18"/>
+      <c r="V46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="W46" s="18"/>
+      <c r="Y46" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z46" s="18"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>0.96799999999999997</v>
       </c>
@@ -2416,12 +2646,16 @@
       <c r="N47" s="1">
         <v>0.94399999999999995</v>
       </c>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="19"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="19"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P47" s="19"/>
+      <c r="Q47" s="20"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="20"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="20"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="20"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>0.92800000000000005</v>
       </c>
@@ -2473,8 +2707,20 @@
       <c r="T48" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W48" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z48" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>0.93600000000000005</v>
       </c>
@@ -2515,19 +2761,27 @@
         <v>0.95199999999999996</v>
       </c>
       <c r="P49" s="10">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="Q49" s="11"/>
+      <c r="S49" s="10">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="T49" s="11"/>
+      <c r="V49" s="10">
         <v>0.87</v>
       </c>
-      <c r="Q49" s="11">
+      <c r="W49" s="11">
         <v>0.88700000000000001</v>
       </c>
-      <c r="S49" s="10">
+      <c r="Y49" s="10">
         <v>0.86199999999999999</v>
       </c>
-      <c r="T49" s="11">
+      <c r="Z49" s="11">
         <v>0.871</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>0.92700000000000005</v>
       </c>
@@ -2568,15 +2822,23 @@
         <v>0.93100000000000005</v>
       </c>
       <c r="P50" s="10">
-        <v>0.879</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="Q50" s="11"/>
       <c r="S50" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="T50" s="11"/>
+      <c r="V50" s="10">
+        <v>0.879</v>
+      </c>
+      <c r="W50" s="11"/>
+      <c r="Y50" s="10">
         <v>0.871</v>
       </c>
-      <c r="T50" s="11"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z50" s="11"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>0.95899999999999996</v>
       </c>
@@ -2617,15 +2879,23 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="P51" s="10">
-        <v>0.878</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="Q51" s="11"/>
       <c r="S51" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="T51" s="11"/>
+      <c r="V51" s="10">
+        <v>0.878</v>
+      </c>
+      <c r="W51" s="11"/>
+      <c r="Y51" s="10">
         <v>0.86199999999999999</v>
       </c>
-      <c r="T51" s="11"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z51" s="11"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>0.96</v>
       </c>
@@ -2666,15 +2936,23 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="P52" s="10">
-        <v>0.879</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="Q52" s="11"/>
       <c r="S52" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="T52" s="11"/>
+      <c r="V52" s="10">
+        <v>0.879</v>
+      </c>
+      <c r="W52" s="11"/>
+      <c r="Y52" s="10">
         <v>0.85599999999999998</v>
       </c>
-      <c r="T52" s="11"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z52" s="11"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>0.95199999999999996</v>
       </c>
@@ -2715,15 +2993,23 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="P53" s="10">
-        <v>0.86899999999999999</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="Q53" s="11"/>
       <c r="S53" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="T53" s="11"/>
+      <c r="V53" s="10">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="W53" s="11"/>
+      <c r="Y53" s="10">
         <v>0.84899999999999998</v>
       </c>
-      <c r="T53" s="11"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z53" s="11"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>0.94299999999999995</v>
       </c>
@@ -2764,15 +3050,23 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="P54" s="10">
-        <v>0.88800000000000001</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="Q54" s="11"/>
       <c r="S54" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="T54" s="11"/>
+      <c r="V54" s="10">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="W54" s="11"/>
+      <c r="Y54" s="10">
         <v>0.87</v>
       </c>
-      <c r="T54" s="11"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z54" s="11"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>0.92700000000000005</v>
       </c>
@@ -2813,15 +3107,23 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="P55" s="10">
-        <v>0.872</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="Q55" s="11"/>
       <c r="S55" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="T55" s="11"/>
+      <c r="V55" s="10">
+        <v>0.872</v>
+      </c>
+      <c r="W55" s="11"/>
+      <c r="Y55" s="10">
         <v>0.85699999999999998</v>
       </c>
-      <c r="T55" s="11"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z55" s="11"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>0.97599999999999998</v>
       </c>
@@ -2862,33 +3164,41 @@
         <v>0.96699999999999997</v>
       </c>
       <c r="P56" s="10">
-        <v>0.88</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="Q56" s="11"/>
       <c r="S56" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="T56" s="11"/>
+      <c r="V56" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="W56" s="11"/>
+      <c r="Y56" s="10">
         <v>0.86199999999999999</v>
       </c>
-      <c r="T56" s="11"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z56" s="11"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <f t="shared" ref="A57:E57" si="19">AVERAGE(A47:A56)</f>
+        <f t="shared" ref="A57:E57" si="22">AVERAGE(A47:A56)</f>
         <v>0.94759999999999989</v>
       </c>
       <c r="B57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.94759999999999989</v>
       </c>
       <c r="C57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.94200000000000017</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.95739999999999981</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.94909999999999994</v>
       </c>
       <c r="F57" s="2">
@@ -2896,75 +3206,107 @@
         <v>0.95083000000000006</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" ref="G57:N57" si="20">AVERAGE(G47:G56)</f>
+        <f t="shared" ref="G57:N57" si="23">AVERAGE(G47:G56)</f>
         <v>0.95500000000000007</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.95350000000000001</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.95530000000000004</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.95299999999999996</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.9588000000000001</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.95410000000000006</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.95550000000000002</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>0.94399999999999995</v>
       </c>
       <c r="P57" s="10">
-        <v>0.872</v>
+        <v>0.8</v>
       </c>
       <c r="Q57" s="11"/>
       <c r="S57" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="T57" s="11"/>
+      <c r="V57" s="10">
+        <v>0.872</v>
+      </c>
+      <c r="W57" s="11"/>
+      <c r="Y57" s="10">
         <v>0.88700000000000001</v>
       </c>
-      <c r="T57" s="11"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Z57" s="11"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P58" s="10">
-        <v>0.89600000000000002</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="Q58" s="11"/>
       <c r="S58" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="T58" s="11"/>
+      <c r="V58" s="10">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="W58" s="11"/>
+      <c r="Y58" s="10">
         <v>0.86399999999999999</v>
       </c>
-      <c r="T58" s="11"/>
-    </row>
-    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z58" s="11"/>
+    </row>
+    <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P59" s="12">
-        <f t="shared" ref="P59:Q59" si="21">AVERAGE(P49:P58)</f>
+        <f t="shared" ref="P59:Q59" si="24">AVERAGE(P49:P58)</f>
+        <v>0.80999999999999994</v>
+      </c>
+      <c r="Q59" s="13" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S59" s="12">
+        <f t="shared" ref="S59:T59" si="25">AVERAGE(S49:S58)</f>
+        <v>0.77340000000000009</v>
+      </c>
+      <c r="T59" s="13" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V59" s="12">
+        <f t="shared" ref="V59:W59" si="26">AVERAGE(V49:V58)</f>
         <v>0.87829999999999997</v>
       </c>
-      <c r="Q59" s="13">
-        <f t="shared" si="21"/>
+      <c r="W59" s="13">
+        <f t="shared" si="26"/>
         <v>0.88700000000000001</v>
       </c>
-      <c r="S59" s="12">
-        <f t="shared" ref="S59:T59" si="22">AVERAGE(S49:S58)</f>
+      <c r="Y59" s="12">
+        <f t="shared" ref="Y59:Z59" si="27">AVERAGE(Y49:Y58)</f>
         <v>0.8640000000000001</v>
       </c>
-      <c r="T59" s="13">
-        <f t="shared" si="22"/>
+      <c r="Z59" s="13">
+        <f t="shared" si="27"/>
         <v>0.871</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -2972,7 +3314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>0</v>
       </c>
@@ -3015,12 +3357,16 @@
       <c r="N61" s="5">
         <v>124</v>
       </c>
-      <c r="P61" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q61" s="17"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P61" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q61" s="18"/>
+      <c r="V61" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W61" s="18"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>0.93600000000000005</v>
       </c>
@@ -3063,10 +3409,12 @@
       <c r="N62" s="1">
         <v>0.96299999999999997</v>
       </c>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="19"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P62" s="19"/>
+      <c r="Q62" s="20"/>
+      <c r="V62" s="19"/>
+      <c r="W62" s="20"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>0.91900000000000004</v>
       </c>
@@ -3112,8 +3460,14 @@
       <c r="Q63" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="W63" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>0.96</v>
       </c>
@@ -3154,13 +3508,17 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="P64" s="10">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q64" s="11"/>
+      <c r="V64" s="10">
         <v>0.84699999999999998</v>
       </c>
-      <c r="Q64" s="11">
+      <c r="W64" s="11">
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>0.97599999999999998</v>
       </c>
@@ -3201,11 +3559,15 @@
         <v>0.97699999999999998</v>
       </c>
       <c r="P65" s="10">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="Q65" s="11"/>
+      <c r="V65" s="10">
         <v>0.879</v>
       </c>
-      <c r="Q65" s="11"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W65" s="11"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>0.90300000000000002</v>
       </c>
@@ -3246,11 +3608,15 @@
         <v>0.96</v>
       </c>
       <c r="P66" s="10">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="Q66" s="11"/>
+      <c r="V66" s="10">
         <v>0.871</v>
       </c>
-      <c r="Q66" s="11"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W66" s="11"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>0.95899999999999996</v>
       </c>
@@ -3291,11 +3657,15 @@
         <v>0.95199999999999996</v>
       </c>
       <c r="P67" s="10">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="Q67" s="11"/>
+      <c r="V67" s="10">
         <v>0.871</v>
       </c>
-      <c r="Q67" s="11"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W67" s="11"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>0.93600000000000005</v>
       </c>
@@ -3336,11 +3706,15 @@
         <v>0.96</v>
       </c>
       <c r="P68" s="10">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="Q68" s="11"/>
+      <c r="V68" s="10">
         <v>0.83099999999999996</v>
       </c>
-      <c r="Q68" s="11"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W68" s="11"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>0.94299999999999995</v>
       </c>
@@ -3381,11 +3755,15 @@
         <v>0.97099999999999997</v>
       </c>
       <c r="P69" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q69" s="11"/>
+      <c r="V69" s="10">
         <v>0.86299999999999999</v>
       </c>
-      <c r="Q69" s="11"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W69" s="11"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>0.94299999999999995</v>
       </c>
@@ -3426,11 +3804,15 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="P70" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q70" s="11"/>
+      <c r="V70" s="10">
         <v>0.85399999999999998</v>
       </c>
-      <c r="Q70" s="11"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W70" s="11"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>0.94299999999999995</v>
       </c>
@@ -3471,29 +3853,33 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="P71" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q71" s="11"/>
+      <c r="V71" s="10">
         <v>0.88700000000000001</v>
       </c>
-      <c r="Q71" s="11"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W71" s="11"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <f t="shared" ref="A72:E72" si="23">AVERAGE(A62:A71)</f>
+        <f t="shared" ref="A72:E72" si="28">AVERAGE(A62:A71)</f>
         <v>0.94179999999999997</v>
       </c>
       <c r="B72" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.95109999999999995</v>
       </c>
       <c r="C72" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.95399999999999996</v>
       </c>
       <c r="D72" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.95489999999999997</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.95550000000000002</v>
       </c>
       <c r="F72" s="2">
@@ -3505,45 +3891,53 @@
         <v>0.95899999999999996</v>
       </c>
       <c r="H72" s="6">
-        <f t="shared" ref="H72:N72" si="24">AVERAGE(H62:H71)</f>
+        <f t="shared" ref="H72:N72" si="29">AVERAGE(H62:H71)</f>
         <v>0.95729999999999982</v>
       </c>
       <c r="I72" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.95389999999999997</v>
       </c>
       <c r="J72" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.95909999999999995</v>
       </c>
       <c r="K72" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.95489999999999997</v>
       </c>
       <c r="L72" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.95299999999999996</v>
       </c>
       <c r="M72" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.96</v>
       </c>
       <c r="N72" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.96299999999999997</v>
       </c>
       <c r="P72" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q72" s="11"/>
+      <c r="V72" s="10">
         <v>0.82099999999999995</v>
       </c>
-      <c r="Q72" s="11"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="W72" s="11"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P73" s="10">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="Q73" s="11"/>
+      <c r="V73" s="10">
         <v>0.86199999999999999</v>
       </c>
-      <c r="Q73" s="11"/>
-    </row>
-    <row r="74" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W73" s="11"/>
+    </row>
+    <row r="74" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -3551,15 +3945,23 @@
         <v>5</v>
       </c>
       <c r="P74" s="12">
-        <f t="shared" ref="P74:Q74" si="25">AVERAGE(P64:P73)</f>
+        <f t="shared" ref="P74:Q74" si="30">AVERAGE(P64:P73)</f>
+        <v>0.81590000000000007</v>
+      </c>
+      <c r="Q74" s="13" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V74" s="12">
+        <f t="shared" ref="V74:W74" si="31">AVERAGE(V64:V73)</f>
         <v>0.85859999999999981</v>
       </c>
-      <c r="Q74" s="13">
-        <f t="shared" si="25"/>
+      <c r="W74" s="13">
+        <f t="shared" si="31"/>
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
@@ -3603,7 +4005,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>0.92700000000000005</v>
       </c>
@@ -3647,7 +4049,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>0.96</v>
       </c>
@@ -3688,7 +4090,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>0.95199999999999996</v>
       </c>
@@ -3729,7 +4131,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>0.95199999999999996</v>
       </c>
@@ -3770,7 +4172,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>0.94299999999999995</v>
       </c>
@@ -4018,23 +4420,23 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <f t="shared" ref="A86:E86" si="26">AVERAGE(A76:A85)</f>
+        <f t="shared" ref="A86:E86" si="32">AVERAGE(A76:A85)</f>
         <v>0.94520000000000004</v>
       </c>
       <c r="B86" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0.94610000000000016</v>
       </c>
       <c r="C86" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0.95579999999999998</v>
       </c>
       <c r="D86" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0.95629999999999993</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0.95429999999999993</v>
       </c>
       <c r="F86" s="2">
@@ -4046,31 +4448,31 @@
         <v>0.95809999999999995</v>
       </c>
       <c r="H86" s="7">
-        <f t="shared" ref="H86:N86" si="27">AVERAGE(H76:H85)</f>
+        <f t="shared" ref="H86:N86" si="33">AVERAGE(H76:H85)</f>
         <v>0.95459999999999989</v>
       </c>
       <c r="I86" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.95989999999999998</v>
       </c>
       <c r="J86" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.95839999999999992</v>
       </c>
       <c r="K86" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.95779999999999998</v>
       </c>
       <c r="L86" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.96479999999999999</v>
       </c>
       <c r="M86" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.96229999999999993</v>
       </c>
       <c r="N86" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.96799999999999997</v>
       </c>
     </row>
@@ -4565,23 +4967,23 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <f t="shared" ref="A100:E100" si="28">AVERAGE(A90:A99)</f>
+        <f t="shared" ref="A100:E100" si="34">AVERAGE(A90:A99)</f>
         <v>0.83379999999999987</v>
       </c>
       <c r="B100" s="7">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.85859999999999981</v>
       </c>
       <c r="C100" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.83050000000000002</v>
       </c>
       <c r="D100" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.81319999999999992</v>
       </c>
       <c r="E100" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0.81340000000000001</v>
       </c>
       <c r="F100" s="2">
@@ -4593,31 +4995,31 @@
         <v>0.81030000000000013</v>
       </c>
       <c r="H100" s="14">
-        <f t="shared" ref="H100:N100" si="29">AVERAGE(H90:H99)</f>
+        <f t="shared" ref="H100:N100" si="35">AVERAGE(H90:H99)</f>
         <v>0.8156000000000001</v>
       </c>
       <c r="I100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.7975000000000001</v>
       </c>
       <c r="J100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.77669999999999995</v>
       </c>
       <c r="K100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.7671</v>
       </c>
       <c r="L100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.75529999999999986</v>
       </c>
       <c r="M100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.70489999999999997</v>
       </c>
       <c r="N100" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0.63550000000000006</v>
       </c>
     </row>
@@ -4715,13 +5117,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="S46:T47"/>
+  <mergeCells count="12">
     <mergeCell ref="P61:Q62"/>
+    <mergeCell ref="P1:Q2"/>
     <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="P1:Q2"/>
     <mergeCell ref="P31:Q32"/>
     <mergeCell ref="P46:Q47"/>
+    <mergeCell ref="S46:T47"/>
+    <mergeCell ref="Y46:Z47"/>
+    <mergeCell ref="V61:W62"/>
+    <mergeCell ref="V16:W17"/>
+    <mergeCell ref="V1:W2"/>
+    <mergeCell ref="V31:W32"/>
+    <mergeCell ref="V46:W47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4729,170 +5137,197 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03A376A-81F2-41B7-A741-EABFFB1024B7}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="16" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.85859999999999981</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.91940000000000011</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="H5" s="15">
         <v>0.95729999999999982</v>
       </c>
-      <c r="B4" s="29">
+      <c r="I5" s="16">
         <v>0.96299999999999997</v>
       </c>
-      <c r="C4" s="15">
-        <v>0.91940000000000011</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="E4" s="15">
+      <c r="J5" s="15">
+        <v>0.8640000000000001</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.871</v>
+      </c>
+      <c r="L5" s="15">
         <v>0.87829999999999997</v>
       </c>
-      <c r="F4" s="15">
+      <c r="M5" s="15">
         <v>0.88700000000000001</v>
       </c>
-      <c r="G4" s="15">
-        <v>0.8640000000000001</v>
-      </c>
-      <c r="H4" s="15">
-        <v>0.871</v>
-      </c>
-      <c r="I4" s="15">
-        <v>0.85859999999999981</v>
-      </c>
-      <c r="J4" s="15">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="K4" s="15">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="L4" s="15">
-        <v>0.83099999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27">
         <v>0.97799999999999998</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="24">
+      <c r="I6" s="28"/>
+      <c r="J6" s="25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="29">
         <v>87.5</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25">
-        <v>0.85</v>
-      </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="L5" s="25"/>
+      <c r="M6" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="K1:L2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E1:F2"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SML Experiment Paper 8/5/2024
</commit_message>
<xml_diff>
--- a/Python/features/DatasetRandomTreeClassificationResults.xlsx
+++ b/Python/features/DatasetRandomTreeClassificationResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\WebApriori\Python\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51220459-5F75-4A64-829A-11AEB6F10648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B323DAF-E35C-4837-B4D6-D907EDCB22F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F99A6A5-D16C-4B5D-A6A4-D283C14BE1EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2F99A6A5-D16C-4B5D-A6A4-D283C14BE1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>K-fold 3</t>
   </si>
@@ -207,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -365,24 +365,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -401,7 +388,18 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -426,33 +424,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -789,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062EC006-8C97-47AC-BD32-415DF786C586}">
   <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>
@@ -799,23 +776,23 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="V1" s="21" t="s">
+      <c r="Q1" s="27"/>
+      <c r="V1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="22"/>
+      <c r="W1" s="27"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="24"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="24"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="29"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1246,23 +1223,23 @@
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="P16" s="17" t="s">
+      <c r="P16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="18"/>
-      <c r="V16" s="17" t="s">
+      <c r="Q16" s="23"/>
+      <c r="V16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="W16" s="18"/>
+      <c r="W16" s="23"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="20"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="20"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="25"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="25"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1896,14 +1873,14 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="P31" s="17" t="s">
+      <c r="P31" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Q31" s="18"/>
-      <c r="V31" s="17" t="s">
+      <c r="Q31" s="23"/>
+      <c r="V31" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="W31" s="18"/>
+      <c r="W31" s="23"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -1948,10 +1925,10 @@
       <c r="N32" s="5">
         <v>120</v>
       </c>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="20"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="20"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="25"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="25"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -2586,22 +2563,22 @@
       <c r="N46" s="5">
         <v>124</v>
       </c>
-      <c r="P46" s="17" t="s">
+      <c r="P46" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q46" s="18"/>
-      <c r="S46" s="17" t="s">
+      <c r="Q46" s="23"/>
+      <c r="S46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T46" s="18"/>
-      <c r="V46" s="17" t="s">
+      <c r="T46" s="23"/>
+      <c r="V46" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="W46" s="18"/>
-      <c r="Y46" s="17" t="s">
+      <c r="W46" s="23"/>
+      <c r="Y46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="Z46" s="18"/>
+      <c r="Z46" s="23"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -2646,14 +2623,14 @@
       <c r="N47" s="1">
         <v>0.94399999999999995</v>
       </c>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="20"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="20"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="20"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="20"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="25"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="25"/>
+      <c r="V47" s="24"/>
+      <c r="W47" s="25"/>
+      <c r="Y47" s="24"/>
+      <c r="Z47" s="25"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -3357,14 +3334,14 @@
       <c r="N61" s="5">
         <v>124</v>
       </c>
-      <c r="P61" s="17" t="s">
+      <c r="P61" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="Q61" s="18"/>
-      <c r="V61" s="17" t="s">
+      <c r="Q61" s="23"/>
+      <c r="V61" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="W61" s="18"/>
+      <c r="W61" s="23"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -3409,10 +3386,10 @@
       <c r="N62" s="1">
         <v>0.96299999999999997</v>
       </c>
-      <c r="P62" s="19"/>
-      <c r="Q62" s="20"/>
-      <c r="V62" s="19"/>
-      <c r="W62" s="20"/>
+      <c r="P62" s="24"/>
+      <c r="Q62" s="25"/>
+      <c r="V62" s="24"/>
+      <c r="W62" s="25"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -5118,11 +5095,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="P61:Q62"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="P31:Q32"/>
-    <mergeCell ref="P46:Q47"/>
     <mergeCell ref="S46:T47"/>
     <mergeCell ref="Y46:Z47"/>
     <mergeCell ref="V61:W62"/>
@@ -5130,6 +5102,11 @@
     <mergeCell ref="V1:W2"/>
     <mergeCell ref="V31:W32"/>
     <mergeCell ref="V46:W47"/>
+    <mergeCell ref="P61:Q62"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="P31:Q32"/>
+    <mergeCell ref="P46:Q47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5137,197 +5114,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03A376A-81F2-41B7-A741-EABFFB1024B7}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32" t="s">
+      <c r="D1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31" t="s">
+      <c r="E1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B4" s="15">
         <v>0.83399999999999996</v>
       </c>
-      <c r="C5" s="15">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C4" s="15">
         <v>0.85859999999999981</v>
       </c>
-      <c r="E5" s="15">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="D4" s="15">
         <v>0.91940000000000011</v>
       </c>
-      <c r="G5" s="15">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="H5" s="15">
+      <c r="E4" s="15">
         <v>0.95729999999999982</v>
       </c>
-      <c r="I5" s="16">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="F4" s="15">
         <v>0.8640000000000001</v>
       </c>
-      <c r="K5" s="15">
-        <v>0.871</v>
-      </c>
-      <c r="L5" s="15">
+      <c r="G4" s="15">
         <v>0.87829999999999997</v>
       </c>
-      <c r="M5" s="15">
-        <v>0.88700000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B5" s="16">
         <v>0.8</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="25">
+      <c r="C5" s="16">
         <v>0.85</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27">
+      <c r="E5" s="17">
         <v>0.97799999999999998</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="25">
+      <c r="F5" s="16">
         <v>0.77500000000000002</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="29">
+      <c r="G5" s="18">
         <v>87.5</v>
       </c>
-      <c r="M6" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F1:G2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
+  <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SML Experiments Paper 9/5/2024
</commit_message>
<xml_diff>
--- a/Python/features/DatasetRandomTreeClassificationResults.xlsx
+++ b/Python/features/DatasetRandomTreeClassificationResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\WebApriori\Python\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B323DAF-E35C-4837-B4D6-D907EDCB22F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B44C76-9621-4670-AF3C-C85085ED6EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2F99A6A5-D16C-4B5D-A6A4-D283C14BE1EA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>K-fold 3</t>
   </si>
@@ -115,6 +115,30 @@
     <t>KNN Classifier
 neighbors=2
 C=1, gamma=0,3</t>
+  </si>
+  <si>
+    <t>SML Algorithm</t>
+  </si>
+  <si>
+    <t>DoD Ver.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 120 instances</t>
+  </si>
+  <si>
+    <t>124 Instances</t>
+  </si>
+  <si>
+    <t>DoD Ver.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>41 instances</t>
+  </si>
+  <si>
+    <t>Training Data</t>
   </si>
 </sst>
 </file>
@@ -369,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -425,10 +449,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5095,6 +5122,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="P61:Q62"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="P16:Q17"/>
+    <mergeCell ref="P31:Q32"/>
+    <mergeCell ref="P46:Q47"/>
     <mergeCell ref="S46:T47"/>
     <mergeCell ref="Y46:Z47"/>
     <mergeCell ref="V61:W62"/>
@@ -5102,11 +5134,6 @@
     <mergeCell ref="V1:W2"/>
     <mergeCell ref="V31:W32"/>
     <mergeCell ref="V46:W47"/>
-    <mergeCell ref="P61:Q62"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="P31:Q32"/>
-    <mergeCell ref="P46:Q47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5114,45 +5141,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03A376A-81F2-41B7-A741-EABFFB1024B7}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -5211,8 +5239,98 @@
         <v>87.5</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>